<commit_message>
Made Changes to run the test case for gmail login
</commit_message>
<xml_diff>
--- a/SAF/src/test/resources/testdata.xlsx
+++ b/SAF/src/test/resources/testdata.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FA38BA3-A0B1-4B6C-9E9C-853200F6CF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -32,9 +33,6 @@
     <t>validateEnteringShipmentID</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -68,24 +66,12 @@
     <t>Test case 1</t>
   </si>
   <si>
-    <t>Test Case 2</t>
-  </si>
-  <si>
     <t>test3</t>
   </si>
   <si>
-    <t>Test Case 3</t>
-  </si>
-  <si>
     <t>valueforsearch</t>
   </si>
   <si>
-    <t>automation</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
     <t>efgh</t>
   </si>
   <si>
@@ -95,25 +81,28 @@
     <t>987</t>
   </si>
   <si>
-    <t>selenium</t>
-  </si>
-  <si>
     <t>hgb1</t>
   </si>
   <si>
     <t>jnh</t>
   </si>
   <si>
-    <t>appium</t>
-  </si>
-  <si>
     <t>test11</t>
+  </si>
+  <si>
+    <t>test12</t>
+  </si>
+  <si>
+    <t>loginTest</t>
+  </si>
+  <si>
+    <t>g.amaresh18@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -152,10 +141,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -175,9 +165,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,9 +205,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,7 +242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -460,11 +450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,61 +475,27 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -548,11 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,27 +522,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -594,71 +550,72 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
+      <c r="D4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="Dhl@1234"/>
-    <hyperlink ref="C3" r:id="rId2" display="Dhl@1234"/>
+    <hyperlink ref="C2" r:id="rId1" display="Dhl@1234" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" display="Dhl@1234" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{24FFE3A5-2ACE-4AF4-9D2B-52CF102A4F04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>